<commit_message>
Completed 2.1 - 2.4
</commit_message>
<xml_diff>
--- a/JavaScriptInfo/javascript_info.xlsx
+++ b/JavaScriptInfo/javascript_info.xlsx
@@ -133,10 +133,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -160,17 +160,11 @@
       <c r="A2" s="0" t="n">
         <v>1.1</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>1.1</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1.2</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>1.2</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -180,6 +174,26 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>1.4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>2.3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>2.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed 2.5 - 2.8
</commit_message>
<xml_diff>
--- a/JavaScriptInfo/javascript_info.xlsx
+++ b/JavaScriptInfo/javascript_info.xlsx
@@ -133,10 +133,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -196,6 +196,21 @@
         <v>2.4</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Upadated 2.10 Logical operators
</commit_message>
<xml_diff>
--- a/JavaScriptInfo/javascript_info.xlsx
+++ b/JavaScriptInfo/javascript_info.xlsx
@@ -136,10 +136,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -229,6 +229,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>2.11</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Completd 2.13 Switch statement
</commit_message>
<xml_diff>
--- a/JavaScriptInfo/javascript_info.xlsx
+++ b/JavaScriptInfo/javascript_info.xlsx
@@ -136,10 +136,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -234,6 +234,11 @@
         <v>2.11</v>
       </c>
     </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>2.13</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added first codewar challenge and completed Javascript.info 2.15
</commit_message>
<xml_diff>
--- a/JavaScriptInfo/javascript_info.xlsx
+++ b/JavaScriptInfo/javascript_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Section 1</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t xml:space="preserve">2_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.15 Function expressions and arrows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16 JavaScript specials</t>
   </si>
 </sst>
 </file>
@@ -136,15 +142,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="19:19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.07"/>
@@ -237,6 +243,16 @@
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>2.13</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed 3.3 and 3.4
</commit_message>
<xml_diff>
--- a/JavaScriptInfo/javascript_info.xlsx
+++ b/JavaScriptInfo/javascript_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Section 1</t>
   </si>
@@ -41,6 +41,15 @@
   </si>
   <si>
     <t xml:space="preserve">3.1 Debugging in Chrome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.2 Coding Style</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.3 Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.4 Ninja code</t>
   </si>
 </sst>
 </file>
@@ -148,10 +157,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -271,6 +280,21 @@
         <v>6</v>
       </c>
     </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Completed 4.5 object primitive converstion and 4.6 constructor new
</commit_message>
<xml_diff>
--- a/JavaScriptInfo/javascript_info.xlsx
+++ b/JavaScriptInfo/javascript_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Section 1</t>
   </si>
@@ -28,6 +28,12 @@
     <t xml:space="preserve">Section 2</t>
   </si>
   <si>
+    <t xml:space="preserve">Down 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Come back to 3.5 Automated testing with Mocha</t>
+  </si>
+  <si>
     <t xml:space="preserve">2_10</t>
   </si>
   <si>
@@ -50,6 +56,15 @@
   </si>
   <si>
     <t xml:space="preserve">3.4 Ninja code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.5 Automated testing with Mocha skipped</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.6 Polyfills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.2 Garbage collection</t>
   </si>
 </sst>
 </file>
@@ -59,7 +74,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -87,6 +102,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,13 +151,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -157,10 +181,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -169,7 +193,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.07"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.85"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -184,6 +209,12 @@
       <c r="A2" s="0" t="n">
         <v>1.1</v>
       </c>
+      <c r="D2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -247,7 +278,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -262,37 +293,52 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactored and reviewed code for 4.6 constructor new
</commit_message>
<xml_diff>
--- a/JavaScriptInfo/javascript_info.xlsx
+++ b/JavaScriptInfo/javascript_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">Section 1</t>
   </si>
@@ -64,13 +64,22 @@
     <t xml:space="preserve">3.6 Polyfills</t>
   </si>
   <si>
+    <t xml:space="preserve">4.1 Objects</t>
+  </si>
+  <si>
     <t xml:space="preserve">4.2 Garbage collection</t>
   </si>
   <si>
+    <t xml:space="preserve">4.3 Symbols skipp for now use a reference</t>
+  </si>
+  <si>
     <t xml:space="preserve">4.5 Object to primitive conversion</t>
   </si>
   <si>
     <t xml:space="preserve">4.6 Constructor, operator “new”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.1 Methods of primitives</t>
   </si>
 </sst>
 </file>
@@ -182,10 +191,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -337,19 +346,34 @@
         <v>13</v>
       </c>
     </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>